<commit_message>
Add Map filed on Hospital.class
</commit_message>
<xml_diff>
--- a/testfileForFileIO/HospitalClassExcel.xlsx
+++ b/testfileForFileIO/HospitalClassExcel.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
   <si>
     <t>hospitalName</t>
   </si>
@@ -50,52 +50,79 @@
     <t>OO1</t>
   </si>
   <si>
+    <t>51</t>
+  </si>
+  <si>
     <t>OO병원2</t>
   </si>
   <si>
     <t>OO2</t>
   </si>
   <si>
+    <t>52</t>
+  </si>
+  <si>
     <t>OO병원3</t>
   </si>
   <si>
     <t>OO3</t>
   </si>
   <si>
+    <t>53</t>
+  </si>
+  <si>
     <t>OO병원4</t>
   </si>
   <si>
     <t>OO4</t>
   </si>
   <si>
+    <t>54</t>
+  </si>
+  <si>
     <t>OO병원5</t>
   </si>
   <si>
     <t>OO5</t>
   </si>
   <si>
+    <t>55</t>
+  </si>
+  <si>
     <t>OO병원6</t>
   </si>
   <si>
     <t>OO6</t>
   </si>
   <si>
+    <t>56</t>
+  </si>
+  <si>
     <t>OO병원7</t>
   </si>
   <si>
     <t>OO7</t>
   </si>
   <si>
+    <t>57</t>
+  </si>
+  <si>
     <t>OO병원8</t>
   </si>
   <si>
     <t>OO8</t>
   </si>
   <si>
+    <t>58</t>
+  </si>
+  <si>
     <t>OO병원9</t>
   </si>
   <si>
     <t>OO9</t>
+  </si>
+  <si>
+    <t>59</t>
   </si>
 </sst>
 </file>
@@ -140,7 +167,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -194,15 +221,15 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -211,15 +238,15 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -228,15 +255,15 @@
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -245,15 +272,15 @@
         <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -262,15 +289,15 @@
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -279,15 +306,15 @@
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -296,15 +323,15 @@
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -313,15 +340,15 @@
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
@@ -330,7 +357,7 @@
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>